<commit_message>
Events updated with Omikron
</commit_message>
<xml_diff>
--- a/data/Events.xlsx
+++ b/data/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sihou\Nextcloud\Studium\TIL Python Programming TIL6022\Project\Group-13---Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA90402-DDAD-481C-80C6-A7F950207D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A964E04-FAD8-4B80-9541-0429DF1CDF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-98" windowWidth="19777" windowHeight="13875" activeTab="1" xr2:uid="{0DD88D09-33D0-4F7E-BA0A-92926894877C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="61">
   <si>
     <t>Date</t>
   </si>
@@ -202,6 +202,24 @@
   </si>
   <si>
     <t>https://www.mdr.de/nachrichten/jahresrueckblick/corona-chronologie-jahresrueckblick-102.html#sprung8</t>
+  </si>
+  <si>
+    <t>Omikron prevalent variant</t>
+  </si>
+  <si>
+    <t>RKI</t>
+  </si>
+  <si>
+    <t>Mitteldeutscher Rundfunk</t>
+  </si>
+  <si>
+    <t>Robert-Koch-Institut</t>
+  </si>
+  <si>
+    <t>https://www.rki.de/DE/Content/InfAZ/N/Neuartiges_Coronavirus/Virusvariante.html</t>
+  </si>
+  <si>
+    <t>Table under the text</t>
   </si>
 </sst>
 </file>
@@ -565,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7884036B-A111-4910-AB0E-59671FE1F09E}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1052,13 +1070,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
-        <v>44593</v>
+        <v>44557</v>
       </c>
       <c r="B39" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C39" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="D39" t="s">
         <v>6</v>
@@ -1066,10 +1084,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
-        <v>44640</v>
+        <v>44593</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C40" t="s">
         <v>10</v>
@@ -1080,15 +1098,29 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
+        <v>44640</v>
+      </c>
+      <c r="B41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A42" s="1">
         <v>44653</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>53</v>
       </c>
-      <c r="C41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="C42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1099,15 +1131,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE641679-B2D0-47EC-88AC-3C15E5CCC747}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1118,40 +1150,40 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1160,6 +1192,20 @@
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>